<commit_message>
commit1 before cycle3 25 aug 2023
</commit_message>
<xml_diff>
--- a/EXCEL_OUPUT/Audited Report Year End March 2023 Final.xlsx
+++ b/EXCEL_OUPUT/Audited Report Year End March 2023 Final.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="921">
   <si>
     <t>Yuan Lee</t>
   </si>
@@ -97,7 +97,7 @@
     <t>the basis of the Financial Report.</t>
   </si>
   <si>
-    <t>A further description of our responsibilities for the audit of the</t>
+    <t>the A further description of our responsibilities for the audit of</t>
   </si>
   <si>
     <t>Auditing and Assurance Standards Boardwebsite at:</t>
@@ -121,7 +121,7 @@
     <t>always detect a material misstatement when it</t>
   </si>
   <si>
-    <t>Financial Report is located at the the</t>
+    <t>the Financial Report is located at the</t>
   </si>
   <si>
     <t>This description forms part of our Auditor's</t>
@@ -295,10 +295,10 @@
     <t>the audit of the Financial Report section of our report.</t>
   </si>
   <si>
-    <t>We 2001 are the independent ethical of the Company in accordance with the Corporations Act and</t>
-  </si>
-  <si>
-    <t>We are independent Code of Ethics requirements of the Accounting Professional and Ethical Standards Board's APES 110</t>
+    <t>2001 the ethical We are independent of the Company in accordance with the Corporations Act and</t>
+  </si>
+  <si>
+    <t>Code We of are Ethics independent requirements of the Accounting Professional and Ethical Standards Board's APES 110</t>
   </si>
   <si>
     <t>for Professional Accountants (including Independence Standards) (the Code) that are relevant</t>
@@ -355,7 +355,7 @@
     <t>The Company is not publicly accountable nor a reporting entity;</t>
   </si>
   <si>
-    <t>The financial statements and notes that as set out on pages 8</t>
+    <t>The 8 financial statements and notes that as set out on pages</t>
   </si>
   <si>
     <t>Act 2001, including:</t>
@@ -382,7 +382,7 @@
     <t>believe that the Company will be able to pay its debts as</t>
   </si>
   <si>
-    <t>to 30 are in accordance with the 8</t>
+    <t>8 to 30 are in accordance with the</t>
   </si>
   <si>
     <t>Corporations</t>
@@ -1450,7 +1450,7 @@
     <t>is</t>
   </si>
   <si>
-    <t>from continuing use that are largely independent of the cash inflows of other assets or CGUS.</t>
+    <t>from of continuing the use cash that inflows are of largely other independent assets or CGUS.</t>
   </si>
   <si>
     <t>amount</t>
@@ -1462,7 +1462,7 @@
     <t>contract</t>
   </si>
   <si>
-    <t>For impairment testing, assets are grouped together into the smailest group of assets that generates cash inflows</t>
+    <t>For cash impairment inflows testing, assets are grouped together into the smailest group of assets that generates</t>
   </si>
   <si>
     <t>An amount. impairment loss is recognised if the carrying amount of an asset or CGU exceeds its recoverable</t>
@@ -1618,7 +1618,7 @@
     <t>expire. The Company also derecognises a financial liability when its terms are modified and the cash flows of the</t>
   </si>
   <si>
-    <t>modified terms liability is are substantially different, in which case a new financial liability based on the modified</t>
+    <t>modified liability are substantially different, in which case a new financial liability based on the modified terms is</t>
   </si>
   <si>
     <t>recognised at fair value.</t>
@@ -2191,52 +2191,121 @@
     <t>policies to ali periods</t>
   </si>
   <si>
-    <t>Accounting</t>
-  </si>
-  <si>
-    <t>Pty</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>are</t>
-  </si>
-  <si>
-    <t>purpose</t>
-  </si>
-  <si>
-    <t>prepared</t>
-  </si>
-  <si>
-    <t>was</t>
-  </si>
-  <si>
-    <t>These</t>
-  </si>
-  <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>2016/191</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>application</t>
+    <t>Note 1 Accounting Policies</t>
+  </si>
+  <si>
+    <t>REPORTING ENTITY</t>
+  </si>
+  <si>
+    <t>Citizen Watches Australia Pty Ltd (the "Company) is domiciled in Australia. The Company's registered office is at Central Plaza Tower 2, Suite 7.01, 475 Victoria Avenue, Chatswood, 2057.</t>
+  </si>
+  <si>
+    <t>The Company is a for-profit entity and is primarily involved in the import and distribution of watches.</t>
+  </si>
+  <si>
+    <t>BASIS OF PREPARATION</t>
+  </si>
+  <si>
+    <t>a) Statement of Compliance</t>
+  </si>
+  <si>
+    <t>These financial statements are general purpose financial statements for distribution to the members and for the</t>
+  </si>
+  <si>
+    <t>purpose of fulfilling the requirements of the Corporations Act 2001. They have been prepared in accordance with</t>
+  </si>
+  <si>
+    <t>Australian Accounting Standards Simplified Disclosures made by the Australian Accounting Standards Board and the Corporations Act 2001.</t>
+  </si>
+  <si>
+    <t>These financial statements are the first general purpose statements prepared in accordance with Australian</t>
+  </si>
+  <si>
+    <t>Accounting Standards Simplified Disclosures. In the</t>
+  </si>
+  <si>
+    <t>financial statements prepared</t>
+  </si>
+  <si>
+    <t>Requirements. There was no impact on the recognition and measurement of amounts recognised in the statements of financial position, profit and loss and other comprehensive income and cash flows of the Company as a result of</t>
+  </si>
+  <si>
+    <t>the change in the basis of preparation.</t>
+  </si>
+  <si>
+    <t>These financial statements were authorised for issue by the Board of Directors as of the date of the Directors</t>
+  </si>
+  <si>
+    <t>Declaration.</t>
+  </si>
+  <si>
+    <t>b) Basis of measurement</t>
+  </si>
+  <si>
+    <t>The financial statements have been prepared on an accruals basis and are based on historical costs unless otherwise</t>
+  </si>
+  <si>
+    <t>stated in the notes.</t>
+  </si>
+  <si>
+    <t>c) Functional and presentation currency and rounding</t>
+  </si>
+  <si>
+    <t>These financial statements are presented in Australian dollars, which is the Company's functional currency. The</t>
+  </si>
+  <si>
+    <t>company is of a kind referred to in ASIC Corporations (Rounding in Financia/Directors' Reports) Instrument</t>
+  </si>
+  <si>
+    <t>2016/191 and in accordance</t>
+  </si>
+  <si>
+    <t>been rounded to the nearest doliar, uniess otherwise indicated.</t>
+  </si>
+  <si>
+    <t>d) Use of judgements and estimates</t>
+  </si>
+  <si>
+    <t>in preparing these financial</t>
+  </si>
+  <si>
+    <t>application of the Company's</t>
   </si>
   <si>
     <t>expenses. Actual results may differ from these estimates.</t>
   </si>
   <si>
-    <t>underlying</t>
-  </si>
-  <si>
-    <t>judgements</t>
-  </si>
-  <si>
-    <t>statements</t>
+    <t>Estimates and underlying assumptions are reviewed on an ongoing basis. Revisions to estimates are recognised prospectively.</t>
+  </si>
+  <si>
+    <t>i. Judgements</t>
+  </si>
+  <si>
+    <t>Information about judgements made in applying accounting policies that have the most significant effects on the amounts recognised in the financial statements is included in the following:</t>
+  </si>
+  <si>
+    <t>lease term: whether the company is reasonably certain to exercise extension options;</t>
+  </si>
+  <si>
+    <t>recognition.</t>
+  </si>
+  <si>
+    <t>in accordance with</t>
+  </si>
+  <si>
+    <t>with that instrument, amounts in the financial statements and directors' report have</t>
+  </si>
+  <si>
+    <t>statements, management has made judgements and estimates that affect the</t>
+  </si>
+  <si>
+    <t>accounting policies and the reported amounts of assets, liabilities, income and</t>
+  </si>
+  <si>
+    <t>prior year the financial statements were general purpose</t>
+  </si>
+  <si>
+    <t>Australian Accounting Standards - Reduced Disclosure</t>
   </si>
   <si>
     <t>CASH FLOWS FROM OPERATING ACTIVITIES</t>
@@ -8724,216 +8793,389 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>546</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B4" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B6" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>714</v>
+      </c>
+      <c r="C6" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B7" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>714</v>
+      </c>
+      <c r="C7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B8" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>715</v>
+      </c>
+      <c r="C8" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B11" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>718</v>
+      </c>
+      <c r="C11" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="B12" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>719</v>
+      </c>
+      <c r="C12" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="B13" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>720</v>
+      </c>
+      <c r="C13" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="B14" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>720</v>
+      </c>
+      <c r="C14" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>715</v>
+        <v>721</v>
       </c>
       <c r="B15" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>721</v>
+      </c>
+      <c r="C15" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>722</v>
+      </c>
       <c r="B16" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>722</v>
+      </c>
+      <c r="C16" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>717</v>
+        <v>723</v>
       </c>
       <c r="B17" t="s">
+        <v>745</v>
+      </c>
+      <c r="C17" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>724</v>
+      </c>
+      <c r="B18" t="s">
+        <v>724</v>
+      </c>
+      <c r="C18" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>724</v>
+      </c>
+      <c r="B19" t="s">
+        <v>724</v>
+      </c>
+      <c r="C19" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>725</v>
+      </c>
+      <c r="B20" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>726</v>
+      </c>
+      <c r="B21" t="s">
+        <v>726</v>
+      </c>
+      <c r="C21" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>718</v>
-      </c>
-      <c r="B18" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>718</v>
-      </c>
-      <c r="B19" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>719</v>
-      </c>
-      <c r="B21" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>463</v>
+        <v>729</v>
       </c>
       <c r="B24" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>729</v>
+      </c>
+      <c r="C24" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>731</v>
+      </c>
+      <c r="B26" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>719</v>
+        <v>732</v>
       </c>
       <c r="B27" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>732</v>
+      </c>
+      <c r="C27" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>720</v>
+        <v>733</v>
       </c>
       <c r="B28" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>733</v>
+      </c>
+      <c r="C28" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>721</v>
+        <v>734</v>
       </c>
       <c r="B29" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>746</v>
+      </c>
+      <c r="C29" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>735</v>
+      </c>
+      <c r="B30" t="s">
+        <v>735</v>
+      </c>
+      <c r="C30" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>736</v>
+      </c>
+      <c r="B31" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>737</v>
+      </c>
+      <c r="B32" t="s">
+        <v>747</v>
+      </c>
+      <c r="C32" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>723</v>
+        <v>738</v>
       </c>
       <c r="B33" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>748</v>
+      </c>
+      <c r="C33" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>739</v>
+      </c>
+      <c r="B34" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>725</v>
+        <v>740</v>
       </c>
       <c r="B35" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>740</v>
+      </c>
+      <c r="C35" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>725</v>
+        <v>740</v>
       </c>
       <c r="B36" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>740</v>
+      </c>
+      <c r="C36" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="B38" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>742</v>
+      </c>
+      <c r="C38" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="B39" t="s">
-        <v>726</v>
+        <v>742</v>
+      </c>
+      <c r="C39" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>743</v>
+      </c>
+      <c r="B40" t="s">
+        <v>743</v>
+      </c>
+      <c r="C40" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -8973,7 +9215,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>748</v>
+        <v>771</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
@@ -8984,34 +9226,34 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>728</v>
+        <v>751</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>729</v>
+        <v>752</v>
       </c>
       <c r="C5" t="s">
-        <v>752</v>
+        <v>775</v>
       </c>
       <c r="D5" t="s">
-        <v>764</v>
+        <v>787</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>730</v>
+        <v>753</v>
       </c>
       <c r="C6" t="s">
-        <v>753</v>
+        <v>776</v>
       </c>
       <c r="D6" t="s">
-        <v>765</v>
+        <v>788</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>731</v>
+        <v>754</v>
       </c>
       <c r="C7" t="s">
         <v>437</v>
@@ -9022,18 +9264,18 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>732</v>
+        <v>755</v>
       </c>
       <c r="C8" t="s">
-        <v>754</v>
+        <v>777</v>
       </c>
       <c r="D8" t="s">
-        <v>766</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>733</v>
+        <v>756</v>
       </c>
       <c r="C9" t="s">
         <v>438</v>
@@ -9044,78 +9286,78 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>734</v>
+        <v>757</v>
       </c>
       <c r="C10" t="s">
-        <v>755</v>
+        <v>778</v>
       </c>
       <c r="D10" t="s">
-        <v>767</v>
+        <v>790</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>735</v>
+        <v>758</v>
       </c>
       <c r="C11" t="s">
-        <v>756</v>
+        <v>779</v>
       </c>
       <c r="D11" t="s">
-        <v>768</v>
+        <v>791</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>736</v>
+        <v>759</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>737</v>
+        <v>760</v>
       </c>
       <c r="B13" t="s">
-        <v>737</v>
+        <v>760</v>
       </c>
       <c r="C13" t="s">
-        <v>757</v>
+        <v>780</v>
       </c>
       <c r="D13" t="s">
-        <v>769</v>
+        <v>792</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>738</v>
+        <v>761</v>
       </c>
       <c r="B14" t="s">
-        <v>749</v>
+        <v>772</v>
       </c>
       <c r="D14" t="s">
-        <v>770</v>
+        <v>793</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>739</v>
+        <v>762</v>
       </c>
       <c r="C15" t="s">
-        <v>757</v>
+        <v>780</v>
       </c>
       <c r="D15" t="s">
-        <v>771</v>
+        <v>794</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>740</v>
+        <v>763</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>741</v>
+        <v>764</v>
       </c>
       <c r="B17" t="s">
-        <v>750</v>
+        <v>773</v>
       </c>
       <c r="C17" t="s">
         <v>236</v>
@@ -9126,71 +9368,71 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>742</v>
+        <v>765</v>
       </c>
       <c r="C18" t="s">
-        <v>758</v>
+        <v>781</v>
       </c>
       <c r="D18" t="s">
-        <v>772</v>
+        <v>795</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>743</v>
+        <v>766</v>
       </c>
       <c r="C19" t="s">
-        <v>759</v>
+        <v>782</v>
       </c>
       <c r="D19" t="s">
-        <v>773</v>
+        <v>796</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>744</v>
+        <v>767</v>
       </c>
       <c r="C20" t="s">
-        <v>760</v>
+        <v>783</v>
       </c>
       <c r="D20" t="s">
-        <v>774</v>
+        <v>797</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>745</v>
+        <v>768</v>
       </c>
       <c r="C21" t="s">
-        <v>761</v>
+        <v>784</v>
       </c>
       <c r="D21" t="s">
-        <v>775</v>
+        <v>798</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>746</v>
+        <v>769</v>
       </c>
       <c r="C22" t="s">
-        <v>762</v>
+        <v>785</v>
       </c>
       <c r="D22" t="s">
-        <v>776</v>
+        <v>799</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>747</v>
+        <v>770</v>
       </c>
       <c r="B23" t="s">
-        <v>751</v>
+        <v>774</v>
       </c>
       <c r="C23" t="s">
-        <v>763</v>
+        <v>786</v>
       </c>
       <c r="D23" t="s">
-        <v>761</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -9222,13 +9464,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>781</v>
+        <v>804</v>
       </c>
       <c r="C2" t="s">
-        <v>783</v>
+        <v>806</v>
       </c>
       <c r="D2" t="s">
-        <v>790</v>
+        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9241,51 +9483,51 @@
         <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
       <c r="C4" t="s">
-        <v>784</v>
+        <v>807</v>
       </c>
       <c r="D4" t="s">
-        <v>791</v>
+        <v>814</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>777</v>
+        <v>800</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>778</v>
+        <v>801</v>
       </c>
       <c r="C6" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
       <c r="D6" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>779</v>
+        <v>802</v>
       </c>
       <c r="C7" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
       <c r="D7" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>780</v>
+        <v>803</v>
       </c>
       <c r="C8" t="s">
-        <v>786</v>
+        <v>809</v>
       </c>
       <c r="D8" t="s">
-        <v>786</v>
+        <v>809</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -9293,51 +9535,51 @@
         <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
       <c r="C9" t="s">
-        <v>787</v>
+        <v>810</v>
       </c>
       <c r="D9" t="s">
-        <v>792</v>
+        <v>815</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>777</v>
+        <v>800</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>778</v>
+        <v>801</v>
       </c>
       <c r="C11" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D11" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>779</v>
+        <v>802</v>
       </c>
       <c r="C12" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D12" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>780</v>
+        <v>803</v>
       </c>
       <c r="C13" t="s">
-        <v>758</v>
+        <v>781</v>
       </c>
       <c r="D13" t="s">
-        <v>758</v>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -9345,13 +9587,13 @@
         <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
       <c r="C14" t="s">
-        <v>789</v>
+        <v>812</v>
       </c>
       <c r="D14" t="s">
-        <v>793</v>
+        <v>816</v>
       </c>
     </row>
   </sheetData>
@@ -9391,7 +9633,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>748</v>
+        <v>771</v>
       </c>
       <c r="C3" t="s">
         <v>121</v>
@@ -9402,48 +9644,48 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>794</v>
+        <v>817</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>795</v>
+        <v>818</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>796</v>
+        <v>819</v>
       </c>
       <c r="B6" t="s">
-        <v>751</v>
+        <v>774</v>
       </c>
       <c r="C6" t="s">
-        <v>763</v>
+        <v>786</v>
       </c>
       <c r="D6" t="s">
-        <v>761</v>
+        <v>784</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>797</v>
+        <v>820</v>
       </c>
       <c r="B7" t="s">
-        <v>821</v>
+        <v>844</v>
       </c>
       <c r="C7" t="s">
-        <v>829</v>
+        <v>852</v>
       </c>
       <c r="D7" t="s">
-        <v>840</v>
+        <v>863</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>798</v>
+        <v>821</v>
       </c>
       <c r="B8" t="s">
-        <v>822</v>
+        <v>845</v>
       </c>
       <c r="C8" t="s">
         <v>322</v>
@@ -9454,37 +9696,37 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>799</v>
+        <v>822</v>
       </c>
       <c r="C9" t="s">
-        <v>830</v>
+        <v>853</v>
       </c>
       <c r="D9" t="s">
-        <v>841</v>
+        <v>864</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>800</v>
+        <v>823</v>
       </c>
       <c r="C10" t="s">
-        <v>831</v>
+        <v>854</v>
       </c>
       <c r="D10" t="s">
-        <v>842</v>
+        <v>865</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>801</v>
+        <v>824</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>802</v>
+        <v>825</v>
       </c>
       <c r="B12" t="s">
-        <v>823</v>
+        <v>846</v>
       </c>
       <c r="C12" t="s">
         <v>379</v>
@@ -9495,10 +9737,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>803</v>
+        <v>826</v>
       </c>
       <c r="B13" t="s">
-        <v>824</v>
+        <v>847</v>
       </c>
       <c r="C13" t="s">
         <v>310</v>
@@ -9509,24 +9751,24 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>804</v>
+        <v>827</v>
       </c>
       <c r="B14" t="s">
-        <v>750</v>
+        <v>773</v>
       </c>
       <c r="C14" t="s">
         <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>843</v>
+        <v>866</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>805</v>
+        <v>828</v>
       </c>
       <c r="B15" t="s">
-        <v>749</v>
+        <v>772</v>
       </c>
       <c r="C15" t="s">
         <v>197</v>
@@ -9537,42 +9779,42 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>806</v>
+        <v>829</v>
       </c>
       <c r="C16" t="s">
-        <v>832</v>
+        <v>855</v>
       </c>
       <c r="D16" t="s">
-        <v>844</v>
+        <v>867</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>807</v>
+        <v>830</v>
       </c>
       <c r="C17" t="s">
-        <v>833</v>
+        <v>856</v>
       </c>
       <c r="D17" t="s">
-        <v>845</v>
+        <v>868</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>808</v>
+        <v>831</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>809</v>
+        <v>832</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>810</v>
+        <v>833</v>
       </c>
       <c r="B20" t="s">
-        <v>825</v>
+        <v>848</v>
       </c>
       <c r="C20" t="s">
         <v>201</v>
@@ -9583,21 +9825,21 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>811</v>
+        <v>834</v>
       </c>
       <c r="C21" t="s">
-        <v>834</v>
+        <v>857</v>
       </c>
       <c r="D21" t="s">
-        <v>846</v>
+        <v>869</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>812</v>
+        <v>835</v>
       </c>
       <c r="B22" t="s">
-        <v>826</v>
+        <v>849</v>
       </c>
       <c r="C22" t="s">
         <v>161</v>
@@ -9608,7 +9850,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="B23" t="s">
-        <v>827</v>
+        <v>850</v>
       </c>
       <c r="C23" t="s">
         <v>163</v>
@@ -9619,40 +9861,40 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>813</v>
+        <v>836</v>
       </c>
       <c r="B24" t="s">
-        <v>750</v>
+        <v>773</v>
       </c>
       <c r="C24" t="s">
-        <v>835</v>
+        <v>858</v>
       </c>
       <c r="D24" t="s">
-        <v>847</v>
+        <v>870</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>814</v>
+        <v>837</v>
       </c>
       <c r="C25" t="s">
-        <v>836</v>
+        <v>859</v>
       </c>
       <c r="D25" t="s">
-        <v>848</v>
+        <v>871</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>815</v>
+        <v>838</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>812</v>
+        <v>835</v>
       </c>
       <c r="B27" t="s">
-        <v>826</v>
+        <v>849</v>
       </c>
       <c r="C27" t="s">
         <v>162</v>
@@ -9663,10 +9905,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>816</v>
+        <v>839</v>
       </c>
       <c r="B28" t="s">
-        <v>827</v>
+        <v>850</v>
       </c>
       <c r="C28" t="s">
         <v>163</v>
@@ -9677,90 +9919,90 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>813</v>
+        <v>836</v>
       </c>
       <c r="B29" t="s">
-        <v>750</v>
+        <v>773</v>
       </c>
       <c r="C29" t="s">
-        <v>837</v>
+        <v>860</v>
       </c>
       <c r="D29" t="s">
-        <v>849</v>
+        <v>872</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>817</v>
+        <v>840</v>
       </c>
       <c r="C30" t="s">
-        <v>838</v>
+        <v>861</v>
       </c>
       <c r="D30" t="s">
-        <v>850</v>
+        <v>873</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>818</v>
+        <v>841</v>
       </c>
       <c r="C31" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="D31" t="s">
-        <v>851</v>
+        <v>874</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>819</v>
+        <v>842</v>
       </c>
       <c r="C32" t="s">
-        <v>793</v>
+        <v>816</v>
       </c>
       <c r="D32" t="s">
-        <v>792</v>
+        <v>815</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>820</v>
+        <v>843</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>781</v>
+        <v>804</v>
       </c>
       <c r="B34" t="s">
-        <v>828</v>
+        <v>851</v>
       </c>
       <c r="C34" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
       <c r="D34" t="s">
-        <v>782</v>
+        <v>805</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>783</v>
+        <v>806</v>
       </c>
       <c r="C35" t="s">
-        <v>789</v>
+        <v>812</v>
       </c>
       <c r="D35" t="s">
-        <v>787</v>
+        <v>810</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>790</v>
+        <v>813</v>
       </c>
       <c r="C36" t="s">
-        <v>793</v>
+        <v>816</v>
       </c>
       <c r="D36" t="s">
-        <v>792</v>
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -9966,7 +10208,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>852</v>
+        <v>875</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -9979,7 +10221,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>748</v>
+        <v>771</v>
       </c>
       <c r="C4" t="s">
         <v>121</v>
@@ -9990,10 +10232,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="B5" t="s">
-        <v>875</v>
+        <v>898</v>
       </c>
       <c r="C5" t="s">
         <v>433</v>
@@ -10004,32 +10246,32 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>854</v>
+        <v>877</v>
       </c>
       <c r="C6" t="s">
-        <v>878</v>
+        <v>901</v>
       </c>
       <c r="D6" t="s">
-        <v>888</v>
+        <v>911</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>855</v>
+        <v>878</v>
       </c>
       <c r="C7" t="s">
-        <v>879</v>
+        <v>902</v>
       </c>
       <c r="D7" t="s">
-        <v>889</v>
+        <v>912</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>856</v>
+        <v>879</v>
       </c>
       <c r="B8" t="s">
-        <v>876</v>
+        <v>899</v>
       </c>
       <c r="C8" t="s">
         <v>436</v>
@@ -10040,87 +10282,87 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>857</v>
+        <v>880</v>
       </c>
       <c r="C9" t="s">
-        <v>880</v>
+        <v>903</v>
       </c>
       <c r="D9" t="s">
-        <v>890</v>
+        <v>913</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>858</v>
+        <v>881</v>
       </c>
       <c r="C10" t="s">
-        <v>881</v>
+        <v>904</v>
       </c>
       <c r="D10" t="s">
-        <v>891</v>
+        <v>914</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>859</v>
+        <v>882</v>
       </c>
       <c r="C11" t="s">
-        <v>882</v>
+        <v>905</v>
       </c>
       <c r="D11" t="s">
-        <v>892</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>860</v>
+        <v>883</v>
       </c>
       <c r="C12" t="s">
-        <v>883</v>
+        <v>906</v>
       </c>
       <c r="D12" t="s">
-        <v>893</v>
+        <v>916</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>861</v>
+        <v>884</v>
       </c>
       <c r="C13" t="s">
-        <v>884</v>
+        <v>907</v>
       </c>
       <c r="D13" t="s">
-        <v>894</v>
+        <v>917</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>862</v>
+        <v>885</v>
       </c>
       <c r="C14" t="s">
-        <v>885</v>
+        <v>908</v>
       </c>
       <c r="D14" t="s">
-        <v>895</v>
+        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>863</v>
+        <v>886</v>
       </c>
       <c r="C15" t="s">
-        <v>886</v>
+        <v>909</v>
       </c>
       <c r="D15" t="s">
-        <v>896</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>864</v>
+        <v>887</v>
       </c>
       <c r="B16" t="s">
-        <v>877</v>
+        <v>900</v>
       </c>
       <c r="C16" t="s">
         <v>437</v>
@@ -10131,10 +10373,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>865</v>
+        <v>888</v>
       </c>
       <c r="B17" t="s">
-        <v>877</v>
+        <v>900</v>
       </c>
       <c r="C17" t="s">
         <v>440</v>
@@ -10145,7 +10387,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>866</v>
+        <v>889</v>
       </c>
       <c r="C18" t="s">
         <v>441</v>
@@ -10156,7 +10398,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>867</v>
+        <v>890</v>
       </c>
       <c r="C19" t="s">
         <v>401</v>
@@ -10167,97 +10409,97 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>868</v>
+        <v>891</v>
       </c>
       <c r="B20" t="s">
-        <v>823</v>
+        <v>846</v>
       </c>
       <c r="C20" t="s">
-        <v>887</v>
+        <v>910</v>
       </c>
       <c r="D20" t="s">
-        <v>897</v>
+        <v>920</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>869</v>
+        <v>892</v>
       </c>
       <c r="C21" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D21" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>870</v>
+        <v>893</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>779</v>
+        <v>802</v>
       </c>
       <c r="C23" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D23" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>871</v>
+        <v>894</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>872</v>
+        <v>895</v>
       </c>
       <c r="C25" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D25" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>869</v>
+        <v>892</v>
       </c>
       <c r="C26" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D26" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>873</v>
+        <v>896</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>872</v>
+        <v>895</v>
       </c>
       <c r="C28" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D28" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>874</v>
+        <v>897</v>
       </c>
       <c r="C29" t="s">
-        <v>788</v>
+        <v>811</v>
       </c>
       <c r="D29" t="s">
-        <v>785</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7 sept office commit: fixed taxes and MCA, MDP issues
</commit_message>
<xml_diff>
--- a/EXCEL_OUPUT/Audited Report Year End March 2023 Final.xlsx
+++ b/EXCEL_OUPUT/Audited Report Year End March 2023 Final.xlsx
@@ -97,7 +97,7 @@
     <t>the basis of the Financial Report.</t>
   </si>
   <si>
-    <t>the A further description of our responsibilities for the audit of</t>
+    <t>A further description of our responsibilities for the audit of the</t>
   </si>
   <si>
     <t>Auditing and Assurance Standards Boardwebsite at:</t>
@@ -121,7 +121,7 @@
     <t>always detect a material misstatement when it</t>
   </si>
   <si>
-    <t>the Financial Report is located at the</t>
+    <t>Financial Report is located at the the</t>
   </si>
   <si>
     <t>This description forms part of our Auditor's</t>
@@ -295,10 +295,10 @@
     <t>the audit of the Financial Report section of our report.</t>
   </si>
   <si>
-    <t>2001 the ethical We are independent of the Company in accordance with the Corporations Act and</t>
-  </si>
-  <si>
-    <t>Code We of are Ethics independent requirements of the Accounting Professional and Ethical Standards Board's APES 110</t>
+    <t>We 2001 are the independent ethical of the Company in accordance with the Corporations Act and</t>
+  </si>
+  <si>
+    <t>We are independent Code of Ethics requirements of the Accounting Professional and Ethical Standards Board's APES 110</t>
   </si>
   <si>
     <t>for Professional Accountants (including Independence Standards) (the Code) that are relevant</t>
@@ -1462,7 +1462,7 @@
     <t>contract</t>
   </si>
   <si>
-    <t>For cash impairment inflows testing, assets are grouped together into the smailest group of assets that generates</t>
+    <t>For impairment testing, assets are grouped together into the smailest group of assets that generates cash inflows</t>
   </si>
   <si>
     <t>An amount. impairment loss is recognised if the carrying amount of an asset or CGU exceeds its recoverable</t>

</xml_diff>